<commit_message>
Added scan-for-skills based on Skillset db for each resume
</commit_message>
<xml_diff>
--- a/output/Report.xlsx
+++ b/output/Report.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\UiPath\SCT9_Diamond_Project2\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336" firstSheet="0" activeTab="0"/>
+    <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <x:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="0"/>
+  <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <x:si>
     <x:t>No.</x:t>
   </x:si>
@@ -31,12 +25,24 @@
     <x:t>Skills</x:t>
   </x:si>
   <x:si>
+    <x:t>URL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Job Ref</x:t>
+  </x:si>
+  <x:si>
     <x:t>Company</x:t>
   </x:si>
   <x:si>
     <x:t>Position</x:t>
   </x:si>
   <x:si>
+    <x:t>Score (%)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gap</x:t>
+  </x:si>
+  <x:si>
     <x:t>Emp Type</x:t>
   </x:si>
   <x:si>
@@ -46,22 +52,13 @@
     <x:t>Industry</x:t>
   </x:si>
   <x:si>
-    <x:t>Score (%)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>URL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Job Ref</x:t>
-  </x:si>
-  <x:si>
     <x:t>Address</x:t>
   </x:si>
   <x:si>
     <x:t>Years</x:t>
   </x:si>
   <x:si>
-    <x:t>Gap</x:t>
+    <x:t>132.pdf</x:t>
   </x:si>
   <x:si>
     <x:t>2.pdf</x:t>
@@ -70,7 +67,25 @@
     <x:t>AutoCAD,Excel,Excellent,MS Office</x:t>
   </x:si>
   <x:si>
+    <x:t>26.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Administration,CRM,Customer Satisfaction,Excel,Excellent</x:t>
+  </x:si>
+  <x:si>
     <x:t>3.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>56.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Communication</x:t>
+  </x:si>
+  <x:si>
+    <x:t>92.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Excel,Excellent,PowerPoint</x:t>
   </x:si>
   <x:si>
     <x:t>Achyuth Resume_8.docx</x:t>
@@ -100,12 +115,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2">
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1" x14ac:knownFonts="1">
+  <x:fonts count="1">
     <x:font>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -121,23 +137,30 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="3">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  <x:cellXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -146,19 +169,10 @@
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
 </x:styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -441,133 +455,168 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A6:C11"/>
+  <x:dimension ref="A1:N11"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="I8" sqref="I8 I8:I8 A1:XFD1048576"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
     <x:row r="1" spans="1:14">
-      <x:c r="A1" s="2" t="s">
+      <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="2" t="s">
+      <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="2" t="s">
+      <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="2" t="s">
+      <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="2" t="s">
+      <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="2" t="s">
+      <x:c r="F1" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="2" t="s">
+      <x:c r="G1" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H1" s="2" t="s">
+      <x:c r="H1" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="I1" s="2" t="s">
+      <x:c r="I1" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="2" t="s">
+      <x:c r="J1" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="K1" s="2" t="s">
+      <x:c r="K1" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="L1" s="2" t="s">
+      <x:c r="L1" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="M1" s="2" t="s">
+      <x:c r="M1" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="N1" s="2" t="s">
+      <x:c r="N1" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:14">
-      <x:c r="A2" s="2" t="n">
+      <x:c r="A2" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B2" s="2" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="C2" s="2" t="s">
+    </x:row>
+    <x:row r="3" spans="1:14">
+      <x:c r="A3" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:14">
-      <x:c r="A3" s="2" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B3" s="2" t="s">
+      <x:c r="C3" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="C3" s="2" t="s">
-        <x:v>15</x:v>
-      </x:c>
     </x:row>
     <x:row r="4" spans="1:14">
-      <x:c r="A4" s="2" t="n">
+      <x:c r="A4" s="0" t="n">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="B4" s="2" t="s">
+      <x:c r="B4" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="C4" s="2" t="s">
+      <x:c r="C4" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:14">
-      <x:c r="A5" s="2" t="n">
+      <x:c r="A5" s="0" t="n">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B5" s="2" t="s">
+      <x:c r="B5" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="C5" s="2" t="s">
+      <x:c r="C5" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:14">
+      <x:c r="A6" s="0" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-    </x:row>
-    <x:row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <x:c r="A6" s="2" t="n">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B6" s="2" t="s">
+      <x:c r="C6" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C6" s="2" t="s">
+    </x:row>
+    <x:row r="7" spans="1:14">
+      <x:c r="A7" s="0" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-    </x:row>
-    <x:row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <x:c r="A7" s="2" t="n">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B7" s="2" t="s">
+      <x:c r="C7" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="C7" s="2" t="s">
+    </x:row>
+    <x:row r="8" spans="1:14">
+      <x:c r="A8" s="0" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-    </x:row>
-    <x:row r="8" spans="1:14" x14ac:dyDescent="0.3"/>
-    <x:row r="9" spans="1:14" x14ac:dyDescent="0.3"/>
-    <x:row r="10" spans="1:14" x14ac:dyDescent="0.3"/>
-    <x:row r="11" spans="1:14" x14ac:dyDescent="0.3"/>
+      <x:c r="C8" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:14">
+      <x:c r="A9" s="0" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:14">
+      <x:c r="A10" s="0" t="n">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:14">
+      <x:c r="A11" s="0" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Refined ReadResume, added Category
</commit_message>
<xml_diff>
--- a/output/Report.xlsx
+++ b/output/Report.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <x:si>
     <x:t>No.</x:t>
   </x:si>
@@ -32,6 +32,9 @@
     <x:t>Skills</x:t>
   </x:si>
   <x:si>
+    <x:t>Category</x:t>
+  </x:si>
+  <x:si>
     <x:t>URL</x:t>
   </x:si>
   <x:si>
@@ -68,55 +71,61 @@
     <x:t>132.pdf</x:t>
   </x:si>
   <x:si>
+    <x:t>English,SEM,TI,Travel</x:t>
+  </x:si>
+  <x:si>
     <x:t>2.pdf</x:t>
   </x:si>
   <x:si>
-    <x:t>AutoCAD,Excel,Excellent,MS Office</x:t>
+    <x:t>AutoCAD,C++,English,Excel,Excellent,MS Office,SEM,TI</x:t>
   </x:si>
   <x:si>
     <x:t>26.pdf</x:t>
   </x:si>
   <x:si>
-    <x:t>Administration,CRM,Customer Satisfaction,Excel,Excellent</x:t>
+    <x:t>Power Point,Administration,CRM,Customer Satisfaction,English,Excel,Excellent,Marketing,Sales,SAP</x:t>
   </x:si>
   <x:si>
     <x:t>3.pdf</x:t>
   </x:si>
   <x:si>
+    <x:t>English,TI</x:t>
+  </x:si>
+  <x:si>
     <x:t>56.pdf</x:t>
   </x:si>
   <x:si>
-    <x:t>Communication</x:t>
+    <x:t>Communication,IP,TI</x:t>
   </x:si>
   <x:si>
     <x:t>92.pdf</x:t>
   </x:si>
   <x:si>
-    <x:t>Excel,Excellent,PowerPoint</x:t>
+    <x:t>PowerPoint,English,Excel,Excellent,TI</x:t>
   </x:si>
   <x:si>
     <x:t>Achyuth Resume_8.docx</x:t>
   </x:si>
   <x:si>
-    <x:t>Agile,Docker,Excel,Excellent,Java,JavaScript,Software Development,SQL,Web Service,Windows</x:t>
+    <x:t>Windows,Agile,Architect,Authorization,Automation,AV,C++,Capital,Customer Service,Databases,Docker,EC2,Excel,Excellent,FX,Healthcare,Java,JavaScript,JIRA,JSON,Linux,Loans,Logging,Mac,Oracle,PL/SQL,Property,Python,SDLC,Servers,Software Development,SQL,Stress,TI,Web Service,XML</x:t>
   </x:si>
   <x:si>
     <x:t>Adelina_Erimia_PMP1.docx</x:t>
   </x:si>
   <x:si>
-    <x:t>Agile,Communication,Construction,Excel,Excellent,ITIL,Leadership,PMP,PowerPoint,project management,Recruiting</x:t>
+    <x:t>PowerPoint,Problem Management,UAT,Agile,Change,Communication,Construction,Consulting,Excel,Excellent,ITIL,Leadership,MS Project,Outlook,PMP,project management,Real Estate,Recruiting,Scrum,SharePoint,TI</x:t>
   </x:si>
   <x:si>
     <x:t>Anil Krishna Mogalaturthi.docx</x:t>
   </x:si>
   <x:si>
-    <x:t>Administration,Agile,Communication,compliance,Docker,Excel,Excellent,Java,JavaScript,Operating Systems,SQL,Troubleshooting,Web Service,Windows</x:t>
+    <x:t>Windows,Administration,Agile,Architect,Automation,AV,Azure,B2B,C++,Communication,compliance,Databases,Docker,EC2,Excel,Excellent,IP,Java,JavaScript,JIRA,JSON,Linux,Logging,Networking,Operating Systems,Oracle,Pipelines,PL/SQL,Scripting,Scrum,SDLC,Selenium,Servers,SQL,System Integration,TI,Troubleshooting,Web Service,XML</x:t>
   </x:si>
   <x:si>
     <x:t>B Shaker-Sr BSA-Scrum Master .docx</x:t>
   </x:si>
   <x:si>
-    <x:t>Agile,compliance,CRM,Excel,Java,JavaScript,MS Office,Operating Systems,SQL,Web Service,Windows</x:t>
+    <x:t>User Acceptance Testing,UAT,Windows,Windows 7,.Net,Accounting,Agile,Assurance,Banking,Business Analyst,Business Requirements,compliance,CRM,Data Migration,Databases,ETL,Excel,Investment Banking,IP,Java,JavaScript,JIRA,Mac,MS Office,MS Project,Operating Systems,Oracle,SAP,Scrum,SDLC,SharePoint,SQL,Tableau,Test Cases,Test Planning,Web Service,XML</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -523,13 +532,19 @@
       <x:c r="N1" s="1" t="s">
         <x:v>13</x:v>
       </x:c>
+      <x:c r="O1" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
     </x:row>
     <x:row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <x:c r="A2" s="1" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C2" s="1" t="s">
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:16" x14ac:dyDescent="0.35">
@@ -537,10 +552,10 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="1" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C3" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:16" x14ac:dyDescent="0.35">
@@ -548,10 +563,10 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="1" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C4" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:16" x14ac:dyDescent="0.35">
@@ -559,10 +574,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C5" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:16" x14ac:dyDescent="0.35">
@@ -570,10 +585,10 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="B6" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C6" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:16" x14ac:dyDescent="0.35">
@@ -581,10 +596,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="1" t="s">
-        <x:v>22</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C7" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:16" x14ac:dyDescent="0.35">
@@ -592,10 +607,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B8" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C8" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:16" x14ac:dyDescent="0.35">
@@ -603,10 +618,10 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C9" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:16" x14ac:dyDescent="0.35">
@@ -614,10 +629,10 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B10" s="1" t="s">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C10" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:16" x14ac:dyDescent="0.35">
@@ -625,10 +640,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
-        <x:v>30</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C11" s="1" t="s">
-        <x:v>31</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:16"/>

</xml_diff>

<commit_message>
Commit job details saved in Report.xlsx
</commit_message>
<xml_diff>
--- a/output/Report.xlsx
+++ b/output/Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tay Hock Gek\Documents\UiPath\sct9-diamond-proj2\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EAC5C1-E133-46F8-AD4D-0CD7CCB46CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBEEA16-798E-4265-A81C-5B692CE87FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <x:si>
     <x:t>No.</x:t>
   </x:si>
@@ -66,6 +66,9 @@
   </x:si>
   <x:si>
     <x:t>Year Exp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Salary</x:t>
   </x:si>
   <x:si>
     <x:t>1388.pdf</x:t>
@@ -238,10 +241,9 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="4">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -550,238 +552,239 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:O5"/>
+  <x:dimension ref="A1:P5"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="E2" sqref="E2 E2:E5"/>
-    </x:sheetView>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:cols>
-    <x:col min="1" max="3" width="8.90625" style="3" customWidth="1"/>
+    <x:col min="1" max="3" width="8.90625" style="2" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <x:c r="A1" s="3" t="s">
+    <x:row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <x:c r="A1" s="2" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="3" t="s">
+      <x:c r="B1" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="3" t="s">
+      <x:c r="C1" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="3" t="s">
+      <x:c r="D1" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="3" t="s">
+      <x:c r="E1" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="3" t="s">
+      <x:c r="F1" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="3" t="s">
+      <x:c r="G1" s="2" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H1" s="3" t="s">
+      <x:c r="H1" s="2" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="I1" s="3" t="s">
+      <x:c r="I1" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="3" t="s">
+      <x:c r="J1" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="K1" s="3" t="s">
+      <x:c r="K1" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="L1" s="3" t="s">
+      <x:c r="L1" s="2" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="M1" s="3" t="s">
+      <x:c r="M1" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="N1" s="3" t="s">
+      <x:c r="N1" s="2" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="O1" s="3" t="s">
+      <x:c r="O1" s="2" t="s">
         <x:v>14</x:v>
       </x:c>
+      <x:c r="P1" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <x:c r="A2" s="3" t="n">
+    <x:row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <x:c r="A2" s="2" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B2" s="3" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C2" s="3" t="s">
+      <x:c r="B2" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="E2" s="3" t="s">
+      <x:c r="C2" s="2" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="F2" s="3" t="s">
+      <x:c r="E2" s="2" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="G2" s="3" t="s">
+      <x:c r="F2" s="2" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="H2" s="3" t="s">
+      <x:c r="G2" s="2" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="I2" s="3" t="s">
+      <x:c r="H2" s="2" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="J2" s="3" t="s">
+      <x:c r="I2" s="2" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="K2" s="3" t="s">
+      <x:c r="J2" s="2" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="L2" s="3" t="s">
+      <x:c r="K2" s="2" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="M2" s="3" t="s">
+      <x:c r="L2" s="2" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="N2" s="3" t="s">
+      <x:c r="M2" s="2" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="O2" s="3" t="s">
+      <x:c r="N2" s="2" t="s">
         <x:v>27</x:v>
       </x:c>
+      <x:c r="O2" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
     </x:row>
-    <x:row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <x:c r="A3" s="3" t="n">
+    <x:row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <x:c r="A3" s="2" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B3" s="3" t="s">
+      <x:c r="B3" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="I3" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="J3" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="K3" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="L3" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="M3" s="2" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="N3" s="2" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="O3" s="2" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="C3" s="3" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E3" s="3" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="F3" s="3" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="G3" s="3" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="H3" s="3" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="I3" s="3" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="J3" s="3" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="K3" s="3" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="L3" s="3" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="M3" s="3" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="N3" s="3" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="O3" s="3" t="s">
+    </x:row>
+    <x:row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <x:c r="A4" s="2" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="F4" s="2" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="H4" s="2" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="I4" s="2" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="J4" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="K4" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="L4" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="M4" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="N4" s="2" t="s">
         <x:v>27</x:v>
       </x:c>
+      <x:c r="O4" s="2" t="s">
+        <x:v>49</x:v>
+      </x:c>
     </x:row>
-    <x:row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <x:c r="A4" s="3" t="n">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B4" s="3" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="C4" s="3" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="E4" s="3" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="F4" s="3" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="G4" s="3" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="H4" s="3" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="I4" s="3" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="J4" s="3" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="K4" s="3" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="L4" s="3" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="M4" s="3" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="N4" s="3" t="s">
+    <x:row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <x:c r="A5" s="2" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="E5" s="2" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="H5" s="2" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="I5" s="2" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="J5" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="K5" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="L5" s="2" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="M5" s="2" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="O4" s="3" t="s">
-        <x:v>48</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <x:c r="A5" s="3" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B5" s="3" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="C5" s="3" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="E5" s="3" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="F5" s="3" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="G5" s="3" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="H5" s="3" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="I5" s="3" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="J5" s="3" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="K5" s="3" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="L5" s="3" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="M5" s="3" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="N5" s="3" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="O5" s="3" t="s">
+      <x:c r="N5" s="2" t="s">
         <x:v>58</x:v>
+      </x:c>
+      <x:c r="O5" s="2" t="s">
+        <x:v>59</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Disable Get OCR Skills Gap - Not working
</commit_message>
<xml_diff>
--- a/output/Report.xlsx
+++ b/output/Report.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <x:si>
     <x:t>No.</x:t>
   </x:si>
@@ -128,9 +128,6 @@
     <x:t xml:space="preserve">Teachers--Physics </x:t>
   </x:si>
   <x:si>
-    <x:t>7% skills matched</x:t>
-  </x:si>
-  <x:si>
     <x:t>Part Time, Full Time</x:t>
   </x:si>
   <x:si>
@@ -161,9 +158,6 @@
     <x:t>Senior Project Manager</x:t>
   </x:si>
   <x:si>
-    <x:t>14% skills matched</x:t>
-  </x:si>
-  <x:si>
     <x:t>Full Time</x:t>
   </x:si>
   <x:si>
@@ -189,9 +183,6 @@
   </x:si>
   <x:si>
     <x:t>GO12267493 - Business Analyst (Contract)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13% skills matched</x:t>
   </x:si>
   <x:si>
     <x:t>Senior Executive</x:t>
@@ -678,22 +669,22 @@
         <x:v>34</x:v>
       </x:c>
       <x:c r="I3" s="2" t="s">
-        <x:v>35</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="J3" s="2" t="s">
         <x:v>23</x:v>
       </x:c>
       <x:c r="K3" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="L3" s="2" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="L3" s="2" t="s">
+      <x:c r="M3" s="2" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="M3" s="2" t="s">
+      <x:c r="N3" s="2" t="s">
         <x:v>38</x:v>
-      </x:c>
-      <x:c r="N3" s="2" t="s">
-        <x:v>39</x:v>
       </x:c>
       <x:c r="O3" s="2" t="s">
         <x:v>28</x:v>
@@ -704,34 +695,34 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="2" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="C4" s="2" t="s">
+      <x:c r="E4" s="2" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="E4" s="2" t="s">
+      <x:c r="F4" s="2" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="F4" s="2" t="s">
+      <x:c r="G4" s="2" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="G4" s="2" t="s">
+      <x:c r="H4" s="2" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="H4" s="2" t="s">
-        <x:v>45</x:v>
-      </x:c>
       <x:c r="I4" s="2" t="s">
-        <x:v>46</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="J4" s="2" t="s">
         <x:v>23</x:v>
       </x:c>
       <x:c r="K4" s="2" t="s">
-        <x:v>47</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="L4" s="2" t="s">
-        <x:v>48</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="M4" s="2" t="s">
         <x:v>26</x:v>
@@ -740,7 +731,7 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="O4" s="2" t="s">
-        <x:v>49</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:16" x14ac:dyDescent="0.35">
@@ -748,25 +739,25 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E5" s="2" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="C5" s="2" t="s">
+      <x:c r="F5" s="2" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="E5" s="2" t="s">
+      <x:c r="G5" s="2" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="F5" s="2" t="s">
+      <x:c r="H5" s="2" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="G5" s="2" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="H5" s="2" t="s">
-        <x:v>55</x:v>
-      </x:c>
       <x:c r="I5" s="2" t="s">
-        <x:v>56</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="J5" s="2" t="s">
         <x:v>23</x:v>
@@ -775,16 +766,16 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="L5" s="2" t="s">
-        <x:v>57</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="M5" s="2" t="s">
         <x:v>26</x:v>
       </x:c>
       <x:c r="N5" s="2" t="s">
-        <x:v>58</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="O5" s="2" t="s">
-        <x:v>59</x:v>
+        <x:v>56</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
I forgot what I updated
</commit_message>
<xml_diff>
--- a/output/Report.xlsx
+++ b/output/Report.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <x:si>
     <x:t>No.</x:t>
   </x:si>
@@ -38,6 +38,18 @@
     <x:t>URL</x:t>
   </x:si>
   <x:si>
+    <x:t>Salary</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1388.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Microsoft Office,PowerPoint,Windows,Windows Operating Systems,Accounting,Construction,Electrical,English,ERP,Excel,ISO,Laboratory,Operating Systems,Pipelines,Wiring</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/manager-wine-trade-asia-18b0eb386bb1cd3491b446f30ee74464</x:t>
+  </x:si>
+  <x:si>
     <x:t>Job Ref</x:t>
   </x:si>
   <x:si>
@@ -47,7 +59,7 @@
     <x:t>Position</x:t>
   </x:si>
   <x:si>
-    <x:t>Score (%)</x:t>
+    <x:t>Score</x:t>
   </x:si>
   <x:si>
     <x:t>Gap</x:t>
@@ -68,37 +80,34 @@
     <x:t>Year Exp</x:t>
   </x:si>
   <x:si>
-    <x:t>Salary</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1388.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Microsoft Office,PowerPoint,Windows,Windows Operating Systems,Accounting,Construction,Electrical,English,ERP,Excel,ISO,Laboratory,Operating Systems,Pipelines,Wiring</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/vm-windows-system-engineer-talento-meld-8b60b4dc412b3473a8ed78118f79cc30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MCF-2022-0291617</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TALENTO MELD PTE. LTD.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VM Windows System Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8% skills matched</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">vSphere, Hardware, VMware, VM, Group Policy, Windows Server, Windows Operating Systems, Problem Management, Configuration Management, Team Player, Software Installation, </x:t>
+    <x:t>64.docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>English,Excel,ICT,ISO,Marketing,Teaching</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.mycareersfuture.gov.sg/job/education-training/specialist-teacher-nexus-international-school-deceab0e66f3121a6ee1decc4db0cdf9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MCF-2022-0272612</x:t>
+  </x:si>
+  <x:si>
+    <x:t>WINE TRADE ASIA PTE. LTD.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IT Manager (6 Months Contract - Renewable  /  Conversion to Full-Time)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40% skills matched</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Troubleshooting, Hardware, Information Technology, Windows Server, Compliance, Technical Support, </x:t>
   </x:si>
   <x:si>
     <x:t>Contract</x:t>
   </x:si>
   <x:si>
-    <x:t>Junior Executive</x:t>
+    <x:t>Manager</x:t>
   </x:si>
   <x:si>
     <x:t>Information Technology</x:t>
@@ -107,109 +116,88 @@
     <x:t>Islandwide</x:t>
   </x:si>
   <x:si>
-    <x:t>2 years exp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>64.docx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>English,Excel,ICT,ISO,Marketing,Teaching</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.mycareersfuture.gov.sg/job/education-training/teachers-physics-vaster-learning-000484fd9bfaf546209b59d94c29c81a</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MCF-2022-0241232</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VASTER LEARNING PTE. LTD.</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Teachers--Physics </x:t>
-  </x:si>
-  <x:si>
-    <x:t>7% skills matched</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">vSphere, Hardware, VMware, VM, Group Policy, Windows Server, Windows Operating Systems, Problem Management, Configuration Management, Team Player, Software Installation, Sports Coaching, Written English, Classroom, Teaching, ICT, Classroom Management, Physics, Tuition, Fitness, International Education, Teaching Experience, Physical Education, Team Player, Manage Change, </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Part Time, Full Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Professional</x:t>
+    <x:t>5 years exp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Adelina_Erimia_PMP1.docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PowerPoint,Problem Management,UAT,Agile,Change,Communication,Construction,Consulting,Excel,ITIL,Leadership,MS Project,Outlook,PMP,project management,Real Estate,Recruiting,Scrum,SharePoint</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/project-manager-trinity-consulting-services-c365ac8714e1c1d4053cb94decc4182a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MCF-2022-0283990</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NEXUS INTERNATIONAL SCHOOL (SINGAPORE) PTE. LTD.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Specialist Teacher</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13% skills matched</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Troubleshooting, Hardware, Information Technology, Windows Server, Compliance, Technical Support, Troubleshooting, Classroom, Teaching, ICT, Social Media, Classroom Management, Attention to Detail, Teaching Experience, Banking, Wellbeing, Evidence, Team Player, Customer Service, </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Non-executive</x:t>
   </x:si>
   <x:si>
     <x:t>Education and Training</x:t>
   </x:si>
   <x:si>
-    <x:t>GOLDHILL SHOPPING CENTRE, 201A THOMSON ROAD 307637</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Adelina_Erimia_PMP1.docx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PowerPoint,Problem Management,UAT,Agile,Change,Communication,Construction,Consulting,Excel,ITIL,Leadership,MS Project,Outlook,PMP,project management,Real Estate,Recruiting,Scrum,SharePoint</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/senior-project-manager-trinity-consulting-services-83635a811c581b8096734efbfd903cb6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MCF-2022-0298794</x:t>
+    <x:t>Nexus International School (Singapore), 01 Aljunied Walk 387293</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3 years exp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SUNITHA Project Manager (1).docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Risk Management,User Acceptance Testing,UAT,Windows,.Net,Active Directory,Agile,Architect,B2B,Business Analyst,Business Intelligence,Change,Data Analysis,Data Migration,Data Modeling,ECC,ERP,ETL,Excel,Healthcare,Java,JavaScript,JIRA,Linux,MS Office,MS Project,Operating Systems,Oracle,Outlook,Payroll,PL/SQL,Power BI,project management,Project Planning,Sales,SAP,SAP BI,SAP HANA,Scheduling,Scrum,SDLC,Servers,SharePoint,SQL,Strategy,Tableau,Technical Design,Test Cases,Time Management,Travel,User Stories,Web Service,XML</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/sap-hr-business-analyst-j37093-scientec-consulting-52d10232dbdd07e9bfa046f379fa4baf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MCF-2022-0064811</x:t>
   </x:si>
   <x:si>
     <x:t>TRINITY CONSULTING SERVICES PTE. LTD.</x:t>
   </x:si>
   <x:si>
-    <x:t>Senior Project Manager</x:t>
-  </x:si>
-  <x:si>
-    <x:t>36% skills matched</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">vSphere, Hardware, VMware, VM, Group Policy, Windows Server, Windows Operating Systems, Problem Management, Configuration Management, Team Player, Software Installation, Sports Coaching, Written English, Classroom, Teaching, ICT, Classroom Management, Physics, Tuition, Fitness, International Education, Teaching Experience, Physical Education, Team Player, Manage Change, Management Skills, Leadership, Construction, Change Management, Program Management, PMP, Project Delivery, Software Development, Business Requirements, </x:t>
+    <x:t>Project Manager</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Troubleshooting, Hardware, Information Technology, Windows Server, Compliance, Technical Support, Troubleshooting, Classroom, Teaching, ICT, Social Media, Classroom Management, Attention to Detail, Teaching Experience, Banking, Wellbeing, Evidence, Team Player, Customer Service, Management Skills, Budgets, Leadership, Construction, Program Management, Compliance, PMP, Team Player, Project Delivery, </x:t>
   </x:si>
   <x:si>
     <x:t>Full Time</x:t>
   </x:si>
   <x:si>
-    <x:t>Manager</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12 years exp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SUNITHA Project Manager (1).docx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Risk Management,User Acceptance Testing,UAT,Windows,.Net,Active Directory,Agile,Architect,B2B,Business Analyst,Business Intelligence,Change,Data Analysis,Data Migration,Data Modeling,ECC,ERP,ETL,Excel,Healthcare,Java,JavaScript,JIRA,Linux,MS Office,MS Project,Operating Systems,Oracle,Outlook,Payroll,PL/SQL,Power BI,project management,Project Planning,Sales,SAP,SAP BI,SAP HANA,Scheduling,Scrum,SDLC,Servers,SharePoint,SQL,Strategy,Tableau,Technical Design,Test Cases,Time Management,Travel,User Stories,Web Service,XML</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/go12267493-business-analyst-robert-half-international-00bbaab076d88a28a130d913f11f5d4a</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MCF-2022-0292701</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ROBERT HALF INTERNATIONAL PTE. LTD.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GO12267493 - Business Analyst (Contract)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>56% skills matched</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">vSphere, Hardware, VMware, VM, Group Policy, Windows Server, Windows Operating Systems, Problem Management, Configuration Management, Team Player, Software Installation, Sports Coaching, Written English, Classroom, Teaching, ICT, Classroom Management, Physics, Tuition, Fitness, International Education, Teaching Experience, Physical Education, Team Player, Manage Change, Management Skills, Leadership, Construction, Change Management, Program Management, PMP, Project Delivery, Software Development, Business Requirements, CRM, Microsoft Excel, Entertainment, Business Analysis, Banking, Team Player, Business Requirements, </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Senior Executive</x:t>
-  </x:si>
-  <x:si>
-    <x:t>REPUBLIC PLAZA, 9 RAFFLES PLACE 048619</x:t>
-  </x:si>
-  <x:si>
     <x:t>7 years exp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MCF-2022-0253781</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SCIENTEC CONSULTING PTE. LTD.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SAP HR Business Analyst - J37093</x:t>
+  </x:si>
+  <x:si>
+    <x:t>41% skills matched</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Troubleshooting, Hardware, Information Technology, Windows Server, Compliance, Technical Support, Troubleshooting, Classroom, Teaching, ICT, Social Media, Classroom Management, Attention to Detail, Teaching Experience, Banking, Wellbeing, Evidence, Team Player, Customer Service, Management Skills, Budgets, Leadership, Construction, Program Management, Compliance, PMP, Team Player, Project Delivery, Workday, Business Analysis, Information Technology, Reliability, SAP HR, Consulting, Business Process, Disaster Recovery, Software Development, Service Delivery, </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Executive</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -244,8 +232,47 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="25">
+  <x:cellStyleXfs count="38">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -659,38 +686,8 @@
       <x:c r="E1" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="2" t="s">
+      <x:c r="P1" s="2" t="s">
         <x:v>5</x:v>
-      </x:c>
-      <x:c r="G1" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="H1" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="I1" s="2" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="J1" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="K1" s="2" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="L1" s="2" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="M1" s="2" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="N1" s="2" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="O1" s="2" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="P1" s="2" t="s">
-        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:16" x14ac:dyDescent="0.35">
@@ -698,43 +695,46 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="B2" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F2" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="G2" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H2" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="I2" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="J2" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="K2" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="L2" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="M2" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="C2" s="2" t="s">
+      <x:c r="N2" s="2" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="E2" s="2" t="s">
+      <x:c r="O2" s="2" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F2" s="2" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G2" s="2" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H2" s="2" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I2" s="2" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="J2" s="3" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="K2" s="2" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="L2" s="2" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="M2" s="2" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="N2" s="2" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="O2" s="2" t="s">
-        <x:v>28</x:v>
+      <x:c r="P2" s="2" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:16" x14ac:dyDescent="0.35">
@@ -742,43 +742,43 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="B3" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E3" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="F3" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="H3" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="I3" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="J3" s="3" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="K3" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L3" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M3" s="2" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="C3" s="2" t="s">
+      <x:c r="N3" s="2" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="E3" s="2" t="s">
+      <x:c r="O3" s="2" t="s">
         <x:v>31</x:v>
-      </x:c>
-      <x:c r="F3" s="2" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="G3" s="2" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="H3" s="2" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="I3" s="2" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="J3" s="3" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="K3" s="2" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="L3" s="2" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="M3" s="2" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="N3" s="2" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="O3" s="2" t="s">
-        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:16" x14ac:dyDescent="0.35">
@@ -786,43 +786,43 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="2" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F4" s="2" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G4" s="2" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="H4" s="2" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="I4" s="2" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="J4" s="3" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="K4" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="L4" s="2" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="M4" s="2" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="C4" s="2" t="s">
+      <x:c r="N4" s="2" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="E4" s="2" t="s">
+      <x:c r="O4" s="2" t="s">
         <x:v>43</x:v>
-      </x:c>
-      <x:c r="F4" s="2" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="G4" s="2" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="H4" s="2" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="I4" s="2" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="J4" s="3" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="K4" s="2" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="L4" s="2" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="M4" s="2" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="N4" s="2" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="O4" s="2" t="s">
-        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:16" x14ac:dyDescent="0.35">
@@ -830,45 +830,91 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B5" s="2" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E5" s="2" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="F5" s="2" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="G5" s="2" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="H5" s="2" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="I5" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="J5" s="3" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="K5" s="2" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L5" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M5" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N5" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="O5" s="2" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="C5" s="2" t="s">
+    </x:row>
+    <x:row r="6" spans="1:16">
+      <x:c r="F6" s="2" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="E5" s="2" t="s">
+      <x:c r="G6" s="2" t="s">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="F5" s="2" t="s">
+      <x:c r="H6" s="2" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="G5" s="2" t="s">
+      <x:c r="I6" s="2" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="H5" s="2" t="s">
+      <x:c r="J6" s="2" t="s">
         <x:v>57</x:v>
       </x:c>
-      <x:c r="I5" s="2" t="s">
+      <x:c r="K6" s="2" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L6" s="2" t="s">
         <x:v>58</x:v>
       </x:c>
-      <x:c r="J5" s="3" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="K5" s="2" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="L5" s="2" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="M5" s="2" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="N5" s="2" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="O5" s="2" t="s">
-        <x:v>62</x:v>
+      <x:c r="M6" s="2" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="N6" s="2" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="O6" s="2" t="s">
+        <x:v>43</x:v>
       </x:c>
     </x:row>
+    <x:row r="7" spans="1:16"/>
+    <x:row r="8" spans="1:16"/>
+    <x:row r="9" spans="1:16"/>
+    <x:row r="10" spans="1:16"/>
+    <x:row r="11" spans="1:16"/>
+    <x:row r="12" spans="1:16"/>
+    <x:row r="13" spans="1:16"/>
+    <x:row r="14" spans="1:16"/>
+    <x:row r="15" spans="1:16"/>
+    <x:row r="16" spans="1:16"/>
+    <x:row r="17" spans="1:16"/>
+    <x:row r="18" spans="1:16"/>
+    <x:row r="19" spans="1:16"/>
+    <x:row r="20" spans="1:16"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Merged GetRecommended and ExtractJobDetails
</commit_message>
<xml_diff>
--- a/output/Report.xlsx
+++ b/output/Report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <x:si>
     <x:t>No.</x:t>
   </x:si>
@@ -70,157 +70,85 @@
     <x:t>Salary</x:t>
   </x:si>
   <x:si>
-    <x:t>1388.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Microsoft Office,PowerPoint,Windows,Windows Operating Systems,Accounting,Construction,Electrical,English,ERP,Excel,ISO,Laboratory,Operating Systems,Pipelines,Wiring</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/vm-windows-system-engineer-es-recruitment-bb7267195028b9ae275a5964fdddbee2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MCF-2022-0293715</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ROVISYS ASIA COMPANY PTE. LTD.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Software Engineer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>47% skills matched</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Rollout, ISO, Software Engineering, Python, Presentation Skills, C#, Software Development, C++, </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Full Time</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fresh/entry level</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Engineering</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Strategy, 2 International Business Park 609930</x:t>
-  </x:si>
-  <x:si>
-    <x:t>64.docx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>English,Excel,ICT,ISO,Marketing,Teaching</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.mycareersfuture.gov.sg/job/education-training/assistant-teacher-blue-house-international-c84cc4dbd83a14aa851573c340659336</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MCF-2022-0292268</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ES RECRUITMENT PTE. LTD.</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">VM Windows System Engineer (Alexandra Rd) </x:t>
-  </x:si>
-  <x:si>
-    <x:t>21% skills matched</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Rollout, ISO, Software Engineering, Python, Presentation Skills, C#, Software Development, C++, Troubleshooting, Windows 10, vSphere, Hardware, Citrix, VMware, VM, Scripting, Group Policy, Windows Server, Windows Operating Systems, Problem Management, Configuration Management, Software Installation, Virtualization, </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Contract</x:t>
+    <x:t>jagadeesh k.docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Windows,Agile,Architect,Architectural,Communication,Data Modeling,Docker,EC2,English,Excel,French,Java,JavaScript,JIRA,JSON,Linux,Networking,Oracle,PL/SQL,project management,Scrum,SDLC,Servers,Software Development,Software Engineering,SQL,Web Service,XML</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/product-development-engineer-forte-employment-services-1a58b2615fc5f3d054a69267a62adf49</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MCF-2022-0299571</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FORTE EMPLOYMENT SERVICES PTE. LTD.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Product Development Engineer (IT /  Java / J2EE / UNIX / $6000)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40% skills matched</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Web Services, Kubernetes, MySQL, Unix, Data Migration, DB2, Web Applications, API, J2EE, </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Permanent</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Manager</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Information Technology</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CT HUB, 2 KALLANG AVENUE 339407</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5 years exp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$3,500 to $6,000 Monthly</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jennifer  M. Conte.docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Windows,Architect,C++,Capital,EC2,Excel,Java,JavaScript,JSON,Linux,Mac,Oracle,SQL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.mycareersfuture.gov.sg/job/engineering/technical-consultant-pacific-tech-8805e8661ff39c929125806c3c632d4d</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MCF-2022-0247090</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PACIFIC TECH PTE. LTD.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Technical Consultant</x:t>
+  </x:si>
+  <x:si>
+    <x:t>43% skills matched</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Leadership, ICT, Dynamics, Selling, Data Migration, Team Player, Software Development, Technical Support, </x:t>
   </x:si>
   <x:si>
     <x:t>Executive</x:t>
   </x:si>
   <x:si>
-    <x:t>Information Technology</x:t>
-  </x:si>
-  <x:si>
-    <x:t>50 TAGORE LANE 787494</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3 years exp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Adelina_Erimia_PMP1.docx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PowerPoint,Problem Management,UAT,Agile,Change,Communication,Construction,Consulting,Excel,ITIL,Leadership,MS Project,Outlook,PMP,project management,Real Estate,Recruiting,Scrum,SharePoint</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/senior-project-manager-trinity-consulting-services-83635a811c581b8096734efbfd903cb6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MCF-2022-0248348</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BLUE HOUSE INTERNATIONAL PTE. LTD.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Assistant Teacher</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0% skills matched</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Rollout, ISO, Software Engineering, Python, Presentation Skills, C#, Software Development, C++, Troubleshooting, Windows 10, vSphere, Hardware, Citrix, VMware, VM, Scripting, Group Policy, Windows Server, Windows Operating Systems, Problem Management, Configuration Management, Software Installation, Virtualization, Childcare, Written English, Classroom, Teaching, Work Well Independently, Stress, Classroom Management, Interpersonal Skills, Early Childhood Education, International Education, Teaching English, First Aid, Teaching Experience, Teaching Children, </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Junior Executive</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Education and Training</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2 TURF CLUB ROAD 287988</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jennifer  M. Conte.docx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Windows,Architect,C++,Capital,EC2,Excel,Java,JavaScript,JSON,Linux,Mac,Oracle,SQL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.mycareersfuture.gov.sg/job/engineering/software-engineer-rovisys-asia-company-eed8074a6f3631baa9767998e6184336</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MCF-2022-0298794</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TRINITY CONSULTING SERVICES PTE. LTD.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Senior Project Manager</x:t>
-  </x:si>
-  <x:si>
-    <x:t>36% skills matched</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Rollout, ISO, Software Engineering, Python, Presentation Skills, C#, Software Development, C++, Troubleshooting, Windows 10, vSphere, Hardware, Citrix, VMware, VM, Scripting, Group Policy, Windows Server, Windows Operating Systems, Problem Management, Configuration Management, Software Installation, Virtualization, Childcare, Written English, Classroom, Teaching, Work Well Independently, Stress, Classroom Management, Interpersonal Skills, Early Childhood Education, International Education, Teaching English, First Aid, Teaching Experience, Teaching Children, Management Skills, Leadership, Construction, Change Management, Program Management, PMP, Project Delivery, Software Development, Business Requirements, </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Manager</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Islandwide</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12 years exp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SUNITHA Project Manager (1).docx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Risk Management,User Acceptance Testing,UAT,Windows,.Net,Active Directory,Agile,Architect,B2B,Business Analyst,Business Intelligence,Change,Data Analysis,Data Migration,Data Modeling,ECC,ERP,ETL,Excel,Healthcare,Java,JavaScript,JIRA,Linux,MS Office,MS Project,Operating Systems,Oracle,Outlook,Payroll,PL/SQL,Power BI,project management,Project Planning,Sales,SAP,SAP BI,SAP HANA,Scheduling,Scrum,SDLC,Servers,SharePoint,SQL,Strategy,Tableau,Technical Design,Test Cases,Time Management,Travel,User Stories,Web Service,XML</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.mycareersfuture.gov.sg/job/banking-finance/business-analyst-financial-markets-encora-technologies-4557eb6061d16fc01228f8b6ed836001</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Rollout, ISO, Software Engineering, Python, Presentation Skills, C#, Software Development, C++, Troubleshooting, Windows 10, vSphere, Hardware, Citrix, VMware, VM, Scripting, Group Policy, Windows Server, Windows Operating Systems, Problem Management, Configuration Management, Software Installation, Virtualization, Childcare, Written English, Classroom, Teaching, Work Well Independently, Stress, Classroom Management, Interpersonal Skills, Early Childhood Education, International Education, Teaching English, First Aid, Teaching Experience, Teaching Children, Management Skills, Leadership, Construction, Change Management, Program Management, PMP, Project Delivery, Software Development, Business Requirements, Rollout, ISO, Software Engineering, Python, Presentation Skills, C#, Software Development, C++, </x:t>
+    <x:t>Engineering, Information Technology</x:t>
+  </x:si>
+  <x:si>
+    <x:t>E-CENTRE @ REDHILL, 3791 JALAN BUKIT MERAH 159471</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2 years exp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$3,800 to $6,000 Monthly</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -255,42 +183,17 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="8">
+  <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="5">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <x:alignment wrapText="1"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -600,281 +503,161 @@
   <x:dimension ref="A1:P6"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A6" sqref="A6 A6:A6 A6:P6"/>
+      <x:selection activeCell="I7" sqref="I7 I7:I7"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:sheetFormatPr defaultColWidth="8.886719" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
-    <x:col min="1" max="3" width="8.886719" style="3" customWidth="1"/>
+    <x:col min="1" max="16384" width="8.886719" style="2" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <x:c r="A1" s="3" t="s">
+      <x:c r="A1" s="2" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="3" t="s">
+      <x:c r="B1" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="3" t="s">
+      <x:c r="C1" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="3" t="s">
+      <x:c r="D1" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="3" t="s">
+      <x:c r="E1" s="2" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="3" t="s">
+      <x:c r="F1" s="2" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="3" t="s">
+      <x:c r="G1" s="2" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H1" s="3" t="s">
+      <x:c r="H1" s="2" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="I1" s="3" t="s">
+      <x:c r="I1" s="2" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="4" t="s">
+      <x:c r="J1" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="K1" s="3" t="s">
+      <x:c r="K1" s="2" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="L1" s="3" t="s">
+      <x:c r="L1" s="2" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="M1" s="3" t="s">
+      <x:c r="M1" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="N1" s="3" t="s">
+      <x:c r="N1" s="2" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="O1" s="3" t="s">
+      <x:c r="O1" s="2" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="P1" s="3" t="s">
+      <x:c r="P1" s="2" t="s">
         <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <x:c r="A2" s="3" t="n">
+      <x:c r="A2" s="2" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B2" s="3" t="s">
+      <x:c r="B2" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="C2" s="3" t="s">
+      <x:c r="C2" s="2" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="E2" s="3" t="s">
+      <x:c r="E2" s="2" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="F2" s="3" t="s">
+      <x:c r="F2" s="2" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="G2" s="3" t="s">
+      <x:c r="G2" s="2" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="H2" s="3" t="s">
+      <x:c r="H2" s="2" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="I2" s="3" t="s">
+      <x:c r="I2" s="2" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="J2" s="3" t="s">
+      <x:c r="J2" s="2" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="K2" s="3" t="s">
+      <x:c r="K2" s="2" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="L2" s="3" t="s">
+      <x:c r="L2" s="2" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="M2" s="3" t="s">
+      <x:c r="M2" s="2" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="N2" s="3" t="s">
+      <x:c r="N2" s="2" t="s">
         <x:v>27</x:v>
+      </x:c>
+      <x:c r="O2" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="P2" s="2" t="s">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <x:c r="A3" s="3" t="n">
+      <x:c r="A3" s="2" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="B3" s="3" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="C3" s="3" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E3" s="3" t="s">
+      <x:c r="B3" s="2" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="F3" s="3" t="s">
+      <x:c r="C3" s="2" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="G3" s="3" t="s">
+      <x:c r="E3" s="2" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="H3" s="3" t="s">
+      <x:c r="F3" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="I3" s="3" t="s">
+      <x:c r="G3" s="2" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="J3" s="4" t="s">
+      <x:c r="H3" s="2" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="K3" s="3" t="s">
+      <x:c r="I3" s="2" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="L3" s="3" t="s">
+      <x:c r="J3" s="2" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="M3" s="3" t="s">
+      <x:c r="K3" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="L3" s="2" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="N3" s="3" t="s">
+      <x:c r="M3" s="2" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="O3" s="3" t="s">
+      <x:c r="N3" s="2" t="s">
         <x:v>40</x:v>
       </x:c>
+      <x:c r="O3" s="2" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="P3" s="2" t="s">
+        <x:v>42</x:v>
+      </x:c>
     </x:row>
-    <x:row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <x:c r="A4" s="3" t="n">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B4" s="3" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C4" s="3" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="E4" s="3" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="F4" s="3" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="G4" s="3" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="H4" s="3" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="I4" s="3" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="J4" s="4" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="K4" s="3" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="L4" s="3" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="M4" s="3" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="N4" s="3" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="O4" s="3" t="s">
-        <x:v>40</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <x:c r="A5" s="3" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B5" s="3" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="C5" s="3" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="E5" s="3" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="F5" s="3" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="G5" s="3" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="H5" s="3" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="I5" s="3" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="J5" s="4" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="K5" s="3" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="L5" s="3" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="M5" s="3" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="N5" s="3" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="O5" s="3" t="s">
-        <x:v>62</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <x:c r="A6" s="3" t="n">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B6" s="3" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="C6" s="3" t="s">
-        <x:v>64</x:v>
-      </x:c>
-      <x:c r="E6" s="3" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="F6" s="3" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="G6" s="3" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="H6" s="3" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="I6" s="3" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="J6" s="3" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="K6" s="3" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="L6" s="3" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="M6" s="3" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="N6" s="3" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="O6" s="3" t="s">
-        <x:v>62</x:v>
-      </x:c>
-    </x:row>
+    <x:row r="4" spans="1:16" x14ac:dyDescent="0.3"/>
+    <x:row r="5" spans="1:16" x14ac:dyDescent="0.3"/>
+    <x:row r="6" spans="1:16" x14ac:dyDescent="0.3"/>
     <x:row r="7" spans="1:16"/>
     <x:row r="8" spans="1:16"/>
     <x:row r="9" spans="1:16"/>

</xml_diff>

<commit_message>
Test success, able to get more than one Recommended
</commit_message>
<xml_diff>
--- a/output/Report.xlsx
+++ b/output/Report.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\UiPath\SCT9_Diamond_Project2\output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="9564" windowHeight="8340" firstSheet="0" activeTab="0"/>
+    <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <x:sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="0"/>
+  <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <x:si>
     <x:t>No.</x:t>
   </x:si>
@@ -31,27 +25,115 @@
     <x:t>Skills</x:t>
   </x:si>
   <x:si>
-    <x:t>Komala BSA Resume.docx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Inventory,Microsoft Office,PowerPoint,Power Point,Risk Management,User Acceptance Testing,UAT,Windows,.Net,Administration,Agile,Architect,Automation,Azure,Business Analyst,Business Requirements,C++,Confluence,Databases,Electrical,Electrical Engineering,ETL,Excel,IIS,Java,JavaScript,JIRA,JSON,Linux,Mac,MS Office,MS Project,Operating Systems,Oracle,Outlook,PL/SQL,Power BI,Property,Scrum,SDLC,Selenium,SharePoint,Software Development,SQL,Strategy,Tableau,Test Cases,Test Strategy,Usability,User Stories,XML</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RaviRaju_Resume.docx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Inventory Management,Inventory,User Acceptance Testing,UAT,Windows,Administration,Agile,Architect,Business Analysis,Business Analyst,Business Intelligence,Business Requirements,Data Analysis,Data Quality,ETL,Excel,Hardware,IIS,IT Operations,ITIL,Java,JavaScript,JIRA,Linux,Network Architecture,Oracle,PMP,Power BI,Publishing,Python,SAP,Scripting,Scrum,SDLC,Servers,Service Desk,SQL,Tableau</x:t>
+    <x:t>Category</x:t>
+  </x:si>
+  <x:si>
+    <x:t>URL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Job Ref</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Company</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Position</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Score</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Gap</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Emp Type</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Job Level</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Job Function</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Year Exp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Salary</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jagadeesh k.docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Windows,Agile,Architect,Architectural,Communication,Data Modeling,Docker,EC2,English,Excel,French,Java,JavaScript,JIRA,JSON,Linux,Networking,Oracle,PL/SQL,project management,Scrum,SDLC,Servers,Software Development,Software Engineering,SQL,Web Service,XML</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/senior-developer-anchor-search-group-27f6977ddf305485b81225727c63b6f1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MCF-2021-0707052</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PRINCESS MANICURE PTE. LTD.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Manicurist / Beauty Therapist</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10% skills matched</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Communication, service oriented, Collaboration, Positive Team Player, Beauty, Salons, Pedicures, Consulting, Manicures, </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Non-executive</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Personal Care / Beauty</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Islandwide</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2 years exp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$2,500 to $3,500 Monthly</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jennifer  M. Conte.docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Windows,Architect,C++,Capital,EC2,Excel,Java,JavaScript,JSON,Linux,Mac,Oracle,SQL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/software-engineer-c-java-flintex-consulting-44ce56bbd4af664f0ad795779bdd8ffa</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SUNITHA Project Manager (1).docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Risk Management,User Acceptance Testing,UAT,Windows,.Net,Active Directory,Agile,Architect,B2B,Business Analyst,Business Intelligence,Data Analysis,Data Migration,Data Modeling,ECC,ERP,ETL,Excel,Healthcare,Java,JavaScript,JIRA,Linux,MS Office,MS Project,Operating Systems,Oracle,Outlook,Payroll,PL/SQL,Power BI,project management,Project Planning,Sales,SAP,SAP BI,SAP HANA,Scheduling,Scrum,SDLC,Servers,SharePoint,SQL,Strategy,Tableau,Technical Design,Test Cases,Time Management,Travel,User Stories,Web Service,XML</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/business-analyst-tech-mahindra-2cd9db73aff974a23e2a51d7bbf65d18</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2">
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1" x14ac:knownFonts="1">
+  <x:fonts count="1">
     <x:font>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -67,22 +149,30 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  <x:cellXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -91,19 +181,10 @@
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
 </x:styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -386,73 +467,307 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <x:sheetPr codeName="Sheet1">
+<file path=xl/worksheets/sheet.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:P99"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <x:pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
-      <x:selection activeCell="C1" sqref="C1 C1:C1"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <x:cols>
-    <x:col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <x:col min="2" max="2" width="35.21875" style="1" customWidth="1"/>
-    <x:col min="3" max="4" width="53.777344" style="1" customWidth="1"/>
-    <x:col min="5" max="5" width="17.21875" style="1" customWidth="1"/>
-    <x:col min="6" max="6" width="49" style="1" customWidth="1"/>
-    <x:col min="7" max="7" width="86.554688" style="1" customWidth="1"/>
-    <x:col min="8" max="8" width="5.664062" style="1" customWidth="1"/>
-    <x:col min="9" max="9" width="53.777344" style="1" customWidth="1"/>
-    <x:col min="10" max="10" width="26.441406" style="1" customWidth="1"/>
-    <x:col min="11" max="11" width="18" style="1" customWidth="1"/>
-    <x:col min="12" max="12" width="75.664062" style="1" customWidth="1"/>
-    <x:col min="13" max="13" width="56.109375" style="1" customWidth="1"/>
-    <x:col min="14" max="14" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="15" max="15" width="24.109375" style="1" customWidth="1"/>
-  </x:cols>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:15">
-      <x:c r="A1" s="1" t="s">
+    <x:row r="1" spans="1:16">
+      <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="1" t="s">
+      <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="1" t="s">
+      <x:c r="C1" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H1" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I1" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="J1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="K1" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="L1" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="M1" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="N1" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="O1" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="P1" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:15">
-      <x:c r="A2" s="1" t="n">
+    <x:row r="2" spans="1:16">
+      <x:c r="A2" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="B2" s="1" t="s">
+      <x:c r="B2" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="K2" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="L2" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="M2" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="N2" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="O2" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="P2" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:16">
+      <x:c r="A3" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="K3" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="L3" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="M3" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="N3" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="O3" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="P3" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:16">
+      <x:c r="A4" s="0" t="n">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="C2" s="1" t="s">
-        <x:v>4</x:v>
+      <x:c r="B4" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="K4" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="L4" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="M4" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="N4" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="O4" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="P4" s="0" t="s">
+        <x:v>29</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:15">
-      <x:c r="A3" s="1" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B3" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C3" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
+    <x:row r="5" spans="1:16"/>
+    <x:row r="6" spans="1:16"/>
+    <x:row r="7" spans="1:16"/>
+    <x:row r="8" spans="1:16"/>
+    <x:row r="9" spans="1:16"/>
+    <x:row r="10" spans="1:16"/>
+    <x:row r="11" spans="1:16"/>
+    <x:row r="12" spans="1:16"/>
+    <x:row r="13" spans="1:16"/>
+    <x:row r="14" spans="1:16"/>
+    <x:row r="15" spans="1:16"/>
+    <x:row r="16" spans="1:16"/>
+    <x:row r="17" spans="1:16"/>
+    <x:row r="18" spans="1:16"/>
+    <x:row r="19" spans="1:16"/>
+    <x:row r="20" spans="1:16"/>
+    <x:row r="21" spans="1:16"/>
+    <x:row r="22" spans="1:16"/>
+    <x:row r="23" spans="1:16"/>
+    <x:row r="24" spans="1:16"/>
+    <x:row r="25" spans="1:16"/>
+    <x:row r="26" spans="1:16"/>
+    <x:row r="27" spans="1:16"/>
+    <x:row r="28" spans="1:16"/>
+    <x:row r="29" spans="1:16"/>
+    <x:row r="30" spans="1:16"/>
+    <x:row r="31" spans="1:16"/>
+    <x:row r="32" spans="1:16"/>
+    <x:row r="33" spans="1:16"/>
+    <x:row r="34" spans="1:16"/>
+    <x:row r="35" spans="1:16"/>
+    <x:row r="36" spans="1:16"/>
+    <x:row r="37" spans="1:16"/>
+    <x:row r="38" spans="1:16"/>
+    <x:row r="39" spans="1:16"/>
+    <x:row r="40" spans="1:16"/>
+    <x:row r="41" spans="1:16"/>
+    <x:row r="42" spans="1:16"/>
+    <x:row r="43" spans="1:16"/>
+    <x:row r="44" spans="1:16"/>
+    <x:row r="45" spans="1:16"/>
+    <x:row r="46" spans="1:16"/>
+    <x:row r="47" spans="1:16"/>
+    <x:row r="48" spans="1:16"/>
+    <x:row r="49" spans="1:16"/>
+    <x:row r="50" spans="1:16"/>
+    <x:row r="51" spans="1:16"/>
+    <x:row r="52" spans="1:16"/>
+    <x:row r="53" spans="1:16"/>
+    <x:row r="54" spans="1:16"/>
+    <x:row r="55" spans="1:16"/>
+    <x:row r="56" spans="1:16"/>
+    <x:row r="57" spans="1:16"/>
+    <x:row r="58" spans="1:16"/>
+    <x:row r="59" spans="1:16"/>
+    <x:row r="60" spans="1:16"/>
+    <x:row r="61" spans="1:16"/>
+    <x:row r="62" spans="1:16"/>
+    <x:row r="63" spans="1:16"/>
+    <x:row r="64" spans="1:16"/>
+    <x:row r="65" spans="1:16"/>
+    <x:row r="66" spans="1:16"/>
+    <x:row r="67" spans="1:16"/>
+    <x:row r="68" spans="1:16"/>
+    <x:row r="69" spans="1:16"/>
+    <x:row r="70" spans="1:16"/>
+    <x:row r="71" spans="1:16"/>
+    <x:row r="72" spans="1:16"/>
+    <x:row r="73" spans="1:16"/>
+    <x:row r="74" spans="1:16"/>
+    <x:row r="75" spans="1:16"/>
+    <x:row r="76" spans="1:16"/>
+    <x:row r="77" spans="1:16"/>
+    <x:row r="78" spans="1:16"/>
+    <x:row r="79" spans="1:16"/>
+    <x:row r="80" spans="1:16"/>
+    <x:row r="81" spans="1:16"/>
+    <x:row r="82" spans="1:16"/>
+    <x:row r="83" spans="1:16"/>
+    <x:row r="84" spans="1:16"/>
+    <x:row r="85" spans="1:16"/>
+    <x:row r="86" spans="1:16"/>
+    <x:row r="87" spans="1:16"/>
+    <x:row r="88" spans="1:16"/>
+    <x:row r="89" spans="1:16"/>
+    <x:row r="90" spans="1:16"/>
+    <x:row r="91" spans="1:16"/>
+    <x:row r="92" spans="1:16"/>
+    <x:row r="93" spans="1:16"/>
+    <x:row r="94" spans="1:16"/>
+    <x:row r="95" spans="1:16"/>
+    <x:row r="96" spans="1:16"/>
+    <x:row r="97" spans="1:16"/>
+    <x:row r="98" spans="1:16"/>
+    <x:row r="99" spans="1:16"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>

</xml_diff>

<commit_message>
Testing to get more than one Recommended
</commit_message>
<xml_diff>
--- a/output/Report.xlsx
+++ b/output/Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <x:si>
     <x:t>No.</x:t>
   </x:si>
@@ -70,49 +70,79 @@
     <x:t>Windows,Agile,Architect,Architectural,Communication,Data Modeling,Docker,EC2,English,Excel,French,Java,JavaScript,JIRA,JSON,Linux,Networking,Oracle,PL/SQL,project management,Scrum,SDLC,Servers,Software Development,Software Engineering,SQL,Web Service,XML</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/senior-developer-anchor-search-group-27f6977ddf305485b81225727c63b6f1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>MCF-2021-0707052</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PRINCESS MANICURE PTE. LTD.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Manicurist / Beauty Therapist</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10% skills matched</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Communication, service oriented, Collaboration, Positive Team Player, Beauty, Salons, Pedicures, Consulting, Manicures, </x:t>
+    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/senior-developer-basil-technologies-0ca878162e09111d2be8ee4a64644aec</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MCF-2022-0296303</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BASIL TECHNOLOGIES PTE. LTD.</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Senior Developer </x:t>
+  </x:si>
+  <x:si>
+    <x:t>56% skills matched</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">SOAP, MySQL, Configuration Management, API, Databases, J2EE, Hibernate, </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contract</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Senior Executive</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Information Technology</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Islandwide</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6 years exp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$6,000 to $8,000 Monthly</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jennifer  M. Conte.docx</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Windows,Architect,C++,Capital,EC2,Excel,Java,JavaScript,JSON,Linux,Mac,Oracle,SQL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.mycareersfuture.gov.sg/job/engineering/senior-software-engineers-marquee-semiconductor-singapore-c62f0f74f24a099da4b542e215d701ac</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MCF-2022-0282201</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MARQUEE SEMICONDUCTOR  SINGAPORE PTE. LTD.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Senior Software Engineers</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30% skills matched</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Version Control, Autonomy, AngularJS, MySQL, Scripting, Information Technology, OpenCL, Requirements Analysis, Python, Computer Architecture, ClearCase, Debugging, Databases, Software Development, </x:t>
   </x:si>
   <x:si>
     <x:t>Full Time</x:t>
   </x:si>
   <x:si>
-    <x:t>Non-executive</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Personal Care / Beauty</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Islandwide</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2 years exp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>$2,500 to $3,500 Monthly</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jennifer  M. Conte.docx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Windows,Architect,C++,Capital,EC2,Excel,Java,JavaScript,JSON,Linux,Mac,Oracle,SQL</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/software-engineer-c-java-flintex-consulting-44ce56bbd4af664f0ad795779bdd8ffa</x:t>
+    <x:t>Middle Management</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Engineering</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1 year exp</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$4,000 to $6,000 Monthly</x:t>
   </x:si>
   <x:si>
     <x:t>SUNITHA Project Manager (1).docx</x:t>
@@ -121,7 +151,31 @@
     <x:t>Risk Management,User Acceptance Testing,UAT,Windows,.Net,Active Directory,Agile,Architect,B2B,Business Analyst,Business Intelligence,Data Analysis,Data Migration,Data Modeling,ECC,ERP,ETL,Excel,Healthcare,Java,JavaScript,JIRA,Linux,MS Office,MS Project,Operating Systems,Oracle,Outlook,Payroll,PL/SQL,Power BI,project management,Project Planning,Sales,SAP,SAP BI,SAP HANA,Scheduling,Scrum,SDLC,Servers,SharePoint,SQL,Strategy,Tableau,Technical Design,Test Cases,Time Management,Travel,User Stories,Web Service,XML</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/business-analyst-tech-mahindra-2cd9db73aff974a23e2a51d7bbf65d18</x:t>
+    <x:t>https://www.mycareersfuture.gov.sg/job/information-technology/business-analyst-5-days-java-2894-supreme-hr-advisory-81fc54813d31f893d647d8ddfa32cb8f</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MCF-2022-0332440</x:t>
+  </x:si>
+  <x:si>
+    <x:t>THE SUPREME HR ADVISORY PTE. LTD.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Business Analyst [5 days| Java] 2894</x:t>
+  </x:si>
+  <x:si>
+    <x:t>50% skills matched</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Requirements Gathering, Microsoft Excel, Business Analysis, Communication Skills, Banking, Web Applications, Team Player, Business Requirements, </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Permanent</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Junior Executive</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$3,200 to $5,000 Monthly</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -589,37 +643,37 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="G3" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="H3" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="I3" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="J3" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="K3" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="L3" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="M3" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="N3" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
       <x:c r="O3" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="P3" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>42</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:16">
@@ -627,34 +681,34 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="I4" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="J4" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="K4" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="L4" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="M4" s="0" t="s">
         <x:v>26</x:v>
@@ -663,10 +717,10 @@
         <x:v>27</x:v>
       </x:c>
       <x:c r="O4" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="P4" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:16"/>

</xml_diff>

<commit_message>
GetRecommended5 - now gets more than one Recommended from the first page
</commit_message>
<xml_diff>
--- a/output/Report.xlsx
+++ b/output/Report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="77">
   <si>
     <t>No.</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Skills</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -75,121 +72,184 @@
     <t>Windows,Agile,Architect,Architectural,Communication,Data Modeling,Docker,EC2,English,Excel,French,Java,JavaScript,JIRA,JSON,Linux,Networking,Oracle,PL/SQL,project management,Scrum,SDLC,Servers,Software Development,Software Engineering,SQL,Web Service,XML</t>
   </si>
   <si>
-    <t>https://www.mycareersfuture.gov.sg/job/information-technology/senior-software-developer-flintex-consulting-2eaf1e57e75b3b7c00c1128200a46f48</t>
-  </si>
-  <si>
-    <t>MCF-2022-0325133</t>
-  </si>
-  <si>
-    <t>FLINTEX CONSULTING PTE. LTD.</t>
-  </si>
-  <si>
-    <t>Senior Software Developer</t>
-  </si>
-  <si>
-    <t>38% skills matched</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MVC, iOS, Web Services, CSS, PHP, Design Patterns, HTML5, SQL Server, Software Design, C#, </t>
+    <t>https://www.mycareersfuture.gov.sg/job/information-technology/software-engineer-commontown-62ceaf29c5989a3494467adc476c1ea2?source=MCF&amp;event=SuggestedJob</t>
+  </si>
+  <si>
+    <t>MCF-2022-0275914</t>
+  </si>
+  <si>
+    <t>COMMONTOWN PRIVATE LIMITED</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Git, Able To Multitask, PHP, MySQL, Python, Applications Support, Software Development, </t>
+  </si>
+  <si>
+    <t>Full Time</t>
+  </si>
+  <si>
+    <t>Senior Executive</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>Vertex (Tower A), 33 Ubi Avenue 3 408868</t>
+  </si>
+  <si>
+    <t>2 years exp</t>
+  </si>
+  <si>
+    <t>$4,000 to $7,000 Monthly</t>
+  </si>
+  <si>
+    <t>https://www.mycareersfuture.gov.sg/job/engineering/senior-product-engineer-lead-digital-gov-solutions-provider-3770-supreme-hr-advisory-134197e72ddf280d04a29b8dad45c76f?source=MCF&amp;event=SuggestedJob</t>
+  </si>
+  <si>
+    <t>MCF-2022-0318306</t>
+  </si>
+  <si>
+    <t>THE SUPREME HR ADVISORY PTE. LTD.</t>
+  </si>
+  <si>
+    <t>Senior Product Engineer  /  Lead - Digital Gov Solutions Provider [3770]</t>
+  </si>
+  <si>
+    <t>25%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MVC, Technical Documentation, Web Services, Kubernetes, Unix, Data Migration, User Acceptance Testing, DB2, Web Applications, J2EE, Software Development, Able To Work Independently, </t>
+  </si>
+  <si>
+    <t>Engineering, Information Technology</t>
+  </si>
+  <si>
+    <t>Islandwide</t>
+  </si>
+  <si>
+    <t>4 years exp</t>
+  </si>
+  <si>
+    <t>$6,800 to $8,800 Monthly</t>
+  </si>
+  <si>
+    <t>Jennifer  M. Conte.docx</t>
+  </si>
+  <si>
+    <t>Windows,Architect,C++,Capital,EC2,Excel,Java,JavaScript,JSON,Linux,Mac,Oracle,SQL</t>
+  </si>
+  <si>
+    <t>https://www.mycareersfuture.gov.sg/job/information-technology/automation-engineer-mavenside-consulting-fb65c956e440d1f6d0538ef688a5e70a?source=MCF&amp;event=SuggestedJob</t>
+  </si>
+  <si>
+    <t>MCF-2022-0315372</t>
+  </si>
+  <si>
+    <t>MAVENSIDE CONSULTING PTE. LTD.</t>
+  </si>
+  <si>
+    <t>IT Automation Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UAT, Scripting, Electrical, Test Cases, PLC, Test Automation, Networking, Python, Selenium, API, S3, Databases, </t>
+  </si>
+  <si>
+    <t>Permanent, Full Time</t>
+  </si>
+  <si>
+    <t>Executive</t>
+  </si>
+  <si>
+    <t>1 year exp</t>
+  </si>
+  <si>
+    <t>$4,500 to $8,000 Monthly</t>
+  </si>
+  <si>
+    <t>https://www.mycareersfuture.gov.sg/job/engineering/software-engineer-rovisys-asia-company-eed8074a6f3631baa9767998e6184336?source=MCF&amp;event=SuggestedJob</t>
+  </si>
+  <si>
+    <t>MCF-2022-0293715</t>
+  </si>
+  <si>
+    <t>ROVISYS ASIA COMPANY PTE. LTD.</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rollout, ISO, Software Engineering, Agile, MS Office, Python, Presentation Skills, C#, Software Development, </t>
+  </si>
+  <si>
+    <t>Fresh/entry level</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Strategy, 2 International Business Park 609930</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>$3,900 to $4,500 Monthly</t>
+  </si>
+  <si>
+    <t>SUNITHA Project Manager (1).docx</t>
+  </si>
+  <si>
+    <t>Risk Management,User Acceptance Testing,UAT,Windows,.Net,Active Directory,Agile,Architect,B2B,Business Analyst,Business Intelligence,Data Analysis,Data Migration,Data Modeling,ECC,ERP,ETL,Excel,Healthcare,Java,JavaScript,JIRA,Linux,MS Office,MS Project,Operating Systems,Oracle,Outlook,Payroll,PL/SQL,Power BI,project management,Project Planning,Sales,SAP,SAP BI,SAP HANA,Scheduling,Scrum,SDLC,Servers,SharePoint,SQL,Strategy,Tableau,Technical Design,Test Cases,Time Management,Travel,User Stories,Web Service,XML</t>
+  </si>
+  <si>
+    <t>https://www.mycareersfuture.gov.sg/job/information-technology/bi-consultant-envoy-search-partners-5b54f64d463cb437ba60f2f5dd2ba944?source=MCF&amp;event=SuggestedJob</t>
+  </si>
+  <si>
+    <t>MCF-2022-0282258</t>
+  </si>
+  <si>
+    <t>ENVOY SEARCH PARTNERS PTE. LIMITED</t>
+  </si>
+  <si>
+    <t>BI Consultant</t>
+  </si>
+  <si>
+    <t>53%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business Analysis, Data Transformation, Advanced Excel, VBA, Information Technology, VBA Programming, Excel VBA, </t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>$4,500 to $7,500 Monthly</t>
+  </si>
+  <si>
+    <t>https://www.mycareersfuture.gov.sg/job/information-technology/business-analyst-5-days-java-2894-supreme-hr-advisory-57f9122e962177ae35d6eaf78e8f8783?source=MCF&amp;event=SuggestedJob</t>
+  </si>
+  <si>
+    <t>MCF-2022-0329028</t>
+  </si>
+  <si>
+    <t>Business Analyst [5 days| Java] 2894</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements Gathering, Microsoft Excel, Business Analysis, Communication Skills, Banking, Web Applications, Team Player, Business Requirements, </t>
   </si>
   <si>
     <t>Permanent</t>
   </si>
   <si>
-    <t>Executive</t>
-  </si>
-  <si>
-    <t>Information Technology</t>
-  </si>
-  <si>
-    <t>INTERNATIONAL PLAZA, 10 ANSON ROAD 079903</t>
-  </si>
-  <si>
-    <t>3 years exp</t>
-  </si>
-  <si>
-    <t>$4,700 to $5,500 Monthly</t>
-  </si>
-  <si>
-    <t>Jennifer  M. Conte.docx</t>
-  </si>
-  <si>
-    <t>Windows,Architect,C++,Capital,EC2,Excel,Java,JavaScript,JSON,Linux,Mac,Oracle,SQL</t>
-  </si>
-  <si>
-    <t>https://www.mycareersfuture.gov.sg/job/engineering/software-engineer-hp-singapore-2cd704771c47b6dd57c425b82ca99713</t>
-  </si>
-  <si>
-    <t>MCF-2022-0278030</t>
-  </si>
-  <si>
-    <t>HP SINGAPORE (PRIVATE) LIMITED</t>
-  </si>
-  <si>
-    <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>33% skills matched</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software Engineering, MySQL, Agile, Python, Team Player, Debugging, API, Databases, Software Development, Human Capital, </t>
-  </si>
-  <si>
-    <t>Permanent, Full Time</t>
-  </si>
-  <si>
     <t>Junior Executive</t>
   </si>
   <si>
-    <t>Engineering, Information Technology</t>
-  </si>
-  <si>
-    <t>1 DEPOT CLOSE 109841</t>
-  </si>
-  <si>
-    <t>2 years exp</t>
-  </si>
-  <si>
-    <t>$4,000 to $6,500 Monthly</t>
-  </si>
-  <si>
-    <t>SUNITHA Project Manager (1).docx</t>
-  </si>
-  <si>
-    <t>Risk Management,User Acceptance Testing,UAT,Windows,.Net,Active Directory,Agile,Architect,B2B,Business Analyst,Business Intelligence,Data Analysis,Data Migration,Data Modeling,ECC,ERP,ETL,Excel,Healthcare,Java,JavaScript,JIRA,Linux,MS Office,MS Project,Operating Systems,Oracle,Outlook,Payroll,PL/SQL,Power BI,project management,Project Planning,Sales,SAP,SAP BI,SAP HANA,Scheduling,Scrum,SDLC,Servers,SharePoint,SQL,Strategy,Tableau,Technical Design,Test Cases,Time Management,Travel,User Stories,Web Service,XML</t>
-  </si>
-  <si>
-    <t>https://www.mycareersfuture.gov.sg/job/information-technology/business-analyst-ijj-recruit-express-287c82d082e493e4dc07b5b3b25c1e6c</t>
-  </si>
-  <si>
-    <t>MCF-2022-0288198</t>
-  </si>
-  <si>
-    <t>RECRUIT EXPRESS PTE LTD</t>
-  </si>
-  <si>
-    <t>IT Business Analyst (no experience is fine, with C#.Net) #IJJ</t>
-  </si>
-  <si>
-    <t>53% skills matched</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change Management, Business Analysis, Information Technology, Banking, Team Player, Business Process, Business Requirements, </t>
-  </si>
-  <si>
-    <t>Contract, Permanent, Full Time</t>
-  </si>
-  <si>
-    <t>Fresh/entry level</t>
-  </si>
-  <si>
-    <t>NGEE ANN CITY, 391A ORCHARD ROAD 238873</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>$3,500 to $4,500 Monthly</t>
+    <t>$3,200 to $5,000 Monthly</t>
   </si>
 </sst>
 </file>
@@ -237,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,18 +305,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,30 +627,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576 E1:E1048576 J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1048576 I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" style="3" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.77734375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="53.77734375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53.77734375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="26.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="42" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" style="5" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.77734375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="53.77734375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="53.77734375" style="8" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="7" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -593,13 +659,13 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -608,13 +674,13 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -629,152 +695,291 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="9"/>
+    </row>
+    <row r="2" spans="1:16" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+    <row r="3" spans="1:16" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="I7" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="M7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="N7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>56</v>
+      <c r="O7" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing GetRecommended6 / Fixing Main, for some reason, it kept moving itself into another folder.
</commit_message>
<xml_diff>
--- a/output/Report.xlsx
+++ b/output/Report.xlsx
@@ -1,106 +1,163 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <x:workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proj\UiPath\SCT9_Diamond_Project2\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="9564" windowHeight="8340" firstSheet="0" activeTab="0"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-  </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="0"/>
-</x:workbook>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9564" windowHeight="8340"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="0"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <x:si>
-    <x:t>No.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Filename</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Skills</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Komala BSA Resume.docx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Inventory,Microsoft Office,PowerPoint,Power Point,Risk Management,User Acceptance Testing,UAT,Windows,.Net,Administration,Agile,Architect,Automation,Azure,Business Analyst,Business Requirements,C++,Confluence,Databases,Electrical,Electrical Engineering,ETL,Excel,IIS,Java,JavaScript,JIRA,JSON,Linux,Mac,MS Office,MS Project,Operating Systems,Oracle,Outlook,PL/SQL,Power BI,Property,Scrum,SDLC,Selenium,SharePoint,Software Development,SQL,Strategy,Tableau,Test Cases,Test Strategy,Usability,User Stories,XML</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RaviRaju_Resume.docx</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Inventory Management,Inventory,User Acceptance Testing,UAT,Windows,Administration,Agile,Architect,Business Analysis,Business Analyst,Business Intelligence,Business Requirements,Data Analysis,Data Quality,ETL,Excel,Hardware,IIS,IT Operations,ITIL,Java,JavaScript,JIRA,Linux,Network Architecture,Oracle,PMP,Power BI,Publishing,Python,SAP,Scripting,Scrum,SDLC,Servers,Service Desk,SQL,Tableau</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Job Ref</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Gap</t>
+  </si>
+  <si>
+    <t>Emp Type</t>
+  </si>
+  <si>
+    <t>Job Level</t>
+  </si>
+  <si>
+    <t>Job Function</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Year Exp</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Komala BSA Resume.docx</t>
+  </si>
+  <si>
+    <t>Inventory,Microsoft Office,PowerPoint,Power Point,Risk Management,User Acceptance Testing,UAT,Windows,.Net,Administration,Agile,Architect,Automation,Azure,Business Analyst,Business Requirements,C++,Confluence,Databases,Electrical,Electrical Engineering,ETL,Excel,IIS,Java,JavaScript,JIRA,JSON,Linux,Mac,MS Office,MS Project,Operating Systems,Oracle,Outlook,PL/SQL,Power BI,Property,Scrum,SDLC,Selenium,SharePoint,Software Development,SQL,Strategy,Tableau,Test Cases,Test Strategy,Usability,User Stories,XML</t>
+  </si>
+  <si>
+    <t>https://www.mycareersfuture.gov.sg/job/information-technology/business-analyst-5-days-java-2894-supreme-hr-advisory-ce6e06b0d3c9285cf81599168925df25</t>
+  </si>
+  <si>
+    <t>MCF-2022-0321842</t>
+  </si>
+  <si>
+    <t>THE SUPREME HR ADVISORY PTE. LTD.</t>
+  </si>
+  <si>
+    <t>Business Analyst [5 days| Java] 2894</t>
+  </si>
+  <si>
+    <t>56%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements Gathering, Microsoft Excel, Business Analysis, Communication Skills, Banking, Web Applications, Team Player, </t>
+  </si>
+  <si>
+    <t>Permanent</t>
+  </si>
+  <si>
+    <t>Junior Executive</t>
+  </si>
+  <si>
+    <t>Information Technology</t>
+  </si>
+  <si>
+    <t>Islandwide</t>
+  </si>
+  <si>
+    <t>1 year exp</t>
+  </si>
+  <si>
+    <t>$3,200 to $5,000 Monthly</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="1" x14ac:knownFonts="1">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellStyleXfs>
-  <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  </cellStyleXfs>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
-</x:styleSheet>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,73 +444,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <x:sheetPr codeName="Sheet1">
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <x:pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
-      <x:selection activeCell="C1" sqref="C1 C1:C1"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <x:cols>
-    <x:col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <x:col min="2" max="2" width="35.21875" style="1" customWidth="1"/>
-    <x:col min="3" max="4" width="53.777344" style="1" customWidth="1"/>
-    <x:col min="5" max="5" width="17.21875" style="1" customWidth="1"/>
-    <x:col min="6" max="6" width="49" style="1" customWidth="1"/>
-    <x:col min="7" max="7" width="86.554688" style="1" customWidth="1"/>
-    <x:col min="8" max="8" width="5.664062" style="1" customWidth="1"/>
-    <x:col min="9" max="9" width="53.777344" style="1" customWidth="1"/>
-    <x:col min="10" max="10" width="26.441406" style="1" customWidth="1"/>
-    <x:col min="11" max="11" width="18" style="1" customWidth="1"/>
-    <x:col min="12" max="12" width="75.664062" style="1" customWidth="1"/>
-    <x:col min="13" max="13" width="56.109375" style="1" customWidth="1"/>
-    <x:col min="14" max="14" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <x:col min="15" max="15" width="24.109375" style="1" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:15">
-      <x:c r="A1" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="1" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:15">
-      <x:c r="A2" s="1" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="B2" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="C2" s="1" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:15">
-      <x:c r="A3" s="1" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B3" s="1" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="C3" s="1" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
+      <selection activeCell="C1" sqref="C1 C1"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.21875" style="1" customWidth="1"/>
+    <col min="3" max="4" width="53.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="49" style="1" customWidth="1"/>
+    <col min="7" max="7" width="86.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="53.77734375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18" style="1" customWidth="1"/>
+    <col min="12" max="12" width="75.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="56.109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sort Report.xlsx based on score, highlight >= 70
</commit_message>
<xml_diff>
--- a/output/Report.xlsx
+++ b/output/Report.xlsx
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$17</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="133">
   <si>
     <t>No.</t>
   </si>
@@ -42,9 +45,6 @@
     <t>Position</t>
   </si>
   <si>
-    <t>Score</t>
-  </si>
-  <si>
     <t>Gap</t>
   </si>
   <si>
@@ -84,9 +84,6 @@
     <t>Business Analyst (Endur)</t>
   </si>
   <si>
-    <t>56%</t>
-  </si>
-  <si>
     <t xml:space="preserve">Microsoft Excel, Analytical Skills, Business Analysis, Project Management, Banking, Team Player, MIS, </t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Software Engineer</t>
   </si>
   <si>
-    <t>69%</t>
-  </si>
-  <si>
     <t xml:space="preserve">Software Engineering, Python, C#, API, MIS, </t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>Business Analyst</t>
   </si>
   <si>
-    <t>75%</t>
-  </si>
-  <si>
     <t xml:space="preserve">Listening Skills, Business Analysis, Agile Methodology, </t>
   </si>
   <si>
@@ -204,9 +195,6 @@
     <t>ITCAN PTE. LIMITED</t>
   </si>
   <si>
-    <t>50%</t>
-  </si>
-  <si>
     <t xml:space="preserve">Microsoft Excel, Analytical Skills, Business Analysis, Information Technology, Project Management, Banking, Team Player, Business Process, </t>
   </si>
   <si>
@@ -243,9 +231,6 @@
     <t>BUSINESS ANALYST</t>
   </si>
   <si>
-    <t>53%</t>
-  </si>
-  <si>
     <t xml:space="preserve">Microsoft Excel, Data Analysis, Business Analysis, Project Management, Banking, Business Process, Integration Testing, </t>
   </si>
   <si>
@@ -273,9 +258,6 @@
     <t>Business Analyst (IT)</t>
   </si>
   <si>
-    <t>47%</t>
-  </si>
-  <si>
     <t xml:space="preserve">Producing, Troubleshooting, User Stories, Information Technology, Project Management, Banking, Presentation Skills, Team Player, </t>
   </si>
   <si>
@@ -297,9 +279,6 @@
     <t>Data Analyst | 12-Months Contract</t>
   </si>
   <si>
-    <t>70%</t>
-  </si>
-  <si>
     <t xml:space="preserve">Critical Thinking, Presentation Skills, Data Analytics, </t>
   </si>
   <si>
@@ -439,6 +418,9 @@
   </si>
   <si>
     <t>$6,000 to $7,000 Monthly</t>
+  </si>
+  <si>
+    <t>Score (%)</t>
   </si>
 </sst>
 </file>
@@ -460,7 +442,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,6 +452,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="44"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -506,6 +494,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -813,28 +804,28 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="C1" sqref="C1 C1"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:D1048576 I1:I1048576"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="23.44140625" style="5" customWidth="1"/>
     <col min="3" max="4" width="53.77734375" style="7" customWidth="1"/>
     <col min="5" max="5" width="18.5546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="49" style="5" customWidth="1"/>
     <col min="7" max="7" width="36" style="5" customWidth="1"/>
-    <col min="8" max="8" width="5.77734375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="53.77734375" style="7" customWidth="1"/>
     <col min="10" max="10" width="19.6640625" style="5" customWidth="1"/>
     <col min="11" max="11" width="15.33203125" style="5" customWidth="1"/>
     <col min="12" max="12" width="41.88671875" style="5" customWidth="1"/>
     <col min="13" max="13" width="54.88671875" style="5" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="5" customWidth="1"/>
     <col min="15" max="15" width="26.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -861,784 +852,787 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>21</v>
+        <v>48</v>
+      </c>
+      <c r="H2" s="8">
+        <v>75</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="J2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="M2" s="5" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" s="8">
+        <v>71</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="8">
+        <v>70</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="L4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="N4" s="5" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="4">
+        <v>69</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" s="5" t="s">
+      <c r="M5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="O5" s="4" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>48</v>
+        <v>117</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>52</v>
+        <v>120</v>
+      </c>
+      <c r="H6" s="4">
+        <v>69</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>55</v>
+        <v>123</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>56</v>
+        <v>124</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>61</v>
+        <v>19</v>
+      </c>
+      <c r="H7" s="4">
+        <v>56</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="L7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="O7" s="4" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>61</v>
+        <v>38</v>
+      </c>
+      <c r="H8" s="4">
+        <v>56</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="J8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="M8" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>74</v>
+        <v>38</v>
+      </c>
+      <c r="H9" s="4">
+        <v>56</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="J9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="M9" s="5" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>84</v>
+        <v>101</v>
+      </c>
+      <c r="H10" s="4">
+        <v>56</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="L10" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="O10" s="4" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>92</v>
+        <v>48</v>
+      </c>
+      <c r="H11" s="4">
+        <v>56</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>94</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="4">
+        <v>53</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="4">
+        <v>50</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="H13" s="4" t="s">
+      <c r="E14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="4">
+        <v>50</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="K14" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>117</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>84</v>
+        <v>92</v>
+      </c>
+      <c r="H15" s="4">
+        <v>50</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>33</v>
+        <v>129</v>
+      </c>
+      <c r="H16" s="4">
+        <v>50</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="O16" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="4">
+        <v>47</v>
+      </c>
+      <c r="I17" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="J17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="N17" s="5" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>139</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:O17">
+    <sortCondition descending="1" ref="H1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>